<commit_message>
Full review of boards - needs NAME still!
</commit_message>
<xml_diff>
--- a/ESP_WiFiDisplay_PCB/ESP_WiFi_Display.xlsx
+++ b/ESP_WiFiDisplay_PCB/ESP_WiFi_Display.xlsx
@@ -409,6 +409,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -430,6 +431,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -481,11 +483,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -531,7 +529,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.77"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.69"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="48.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="67.29"/>
@@ -539,7 +537,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="10.19"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="125.51"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="14.49"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="16.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="16.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="19.36"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="11" style="0" width="11.52"/>
   </cols>
@@ -1191,7 +1189,7 @@
       <c r="F34" s="0" t="s">
         <v>112</v>
       </c>
-      <c r="H34" s="1" t="n">
+      <c r="H34" s="0" t="n">
         <v>3</v>
       </c>
     </row>
@@ -1264,22 +1262,22 @@
         <v>5</v>
       </c>
     </row>
-    <row r="44" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="2" t="s">
+    <row r="44" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="B44" s="2" t="s">
+      <c r="B44" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="H44" s="2" t="n">
+      <c r="H44" s="1" t="n">
         <v>5</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G45" s="3" t="s">
+      <c r="G45" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="H45" s="4" t="n">
+      <c r="H45" s="3" t="n">
         <f aca="false">SUM(H2:H44)</f>
         <v>29.38</v>
       </c>

</xml_diff>